<commit_message>
see if explicitly classifying xls/xlsx as binary files helps
</commit_message>
<xml_diff>
--- a/data_capture/static/data_capture/s736_example.xlsx
+++ b/data_capture/static/data_capture/s736_example.xlsx
@@ -1,16 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27011"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/heatherbattaglia/Projects/calc/data_capture/static/data_capture/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2535" yWindow="4920" windowWidth="20370" windowHeight="8655"/>
+    <workbookView xWindow="2540" yWindow="4920" windowWidth="20380" windowHeight="8660"/>
   </bookViews>
   <sheets>
     <sheet name="Professional Market Prce Escala" sheetId="1" r:id="rId1"/>
     <sheet name="Professional Commer Price Escla" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -108,9 +121,6 @@
   </si>
   <si>
     <t>Junior Analyst</t>
-  </si>
-  <si>
-    <t>BA/BS</t>
   </si>
   <si>
     <t>Hour</t>
@@ -217,6 +227,9 @@
   </si>
   <si>
     <t>7FCM-N6-030736-B Refresh 30</t>
+  </si>
+  <si>
+    <t>Bachelors</t>
   </si>
 </sst>
 </file>
@@ -357,16 +370,16 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -621,12 +634,12 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -656,12 +669,12 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -867,27 +880,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:F1"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="18" width="8.88671875" style="43"/>
-    <col min="19" max="19" width="9.44140625" style="43" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.44140625" style="43" bestFit="1" customWidth="1"/>
+    <col min="1" max="18" width="8.85546875" style="43"/>
+    <col min="19" max="19" width="9.42578125" style="43" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.42578125" style="43" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="15" style="43" bestFit="1" customWidth="1"/>
-    <col min="22" max="16384" width="8.88671875" style="43"/>
+    <col min="22" max="16384" width="8.85546875" style="43"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A1" s="49" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="49"/>
       <c r="C1" s="44"/>
       <c r="D1" s="49" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E1" s="49"/>
       <c r="F1" s="49"/>
@@ -1142,7 +1155,7 @@
         <v>30</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>31</v>
+        <v>58</v>
       </c>
       <c r="D12" s="1">
         <v>2</v>
@@ -1151,10 +1164,10 @@
         <v>50</v>
       </c>
       <c r="F12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G12" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>33</v>
       </c>
       <c r="H12" s="3">
         <v>0</v>
@@ -1163,7 +1176,7 @@
         <v>50</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K12" s="3">
         <v>0.15</v>
@@ -1227,16 +1240,16 @@
       <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" s="50" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="50"/>
       <c r="C1" s="31"/>
       <c r="D1" s="50" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E1" s="50"/>
       <c r="F1" s="50"/>
@@ -1391,83 +1404,83 @@
       <c r="O9" s="5"/>
       <c r="P9" s="5"/>
     </row>
-    <row r="12" spans="1:16" ht="56.25" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" ht="55" x14ac:dyDescent="0.2">
       <c r="A12" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="B12" s="23" t="s">
+      <c r="C12" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="23" t="s">
+      <c r="D12" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="D12" s="24" t="s">
+      <c r="E12" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="E12" s="24" t="s">
+      <c r="F12" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="F12" s="24" t="s">
+      <c r="G12" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="G12" s="25" t="s">
+      <c r="H12" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="H12" s="23" t="s">
+      <c r="I12" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="I12" s="23" t="s">
+      <c r="J12" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="J12" s="26" t="s">
+      <c r="K12" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="K12" s="27" t="s">
+      <c r="L12" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="L12" s="28" t="s">
+      <c r="M12" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="M12" s="27" t="s">
+      <c r="N12" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="N12" s="29" t="s">
+      <c r="O12" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="O12" s="27" t="s">
+      <c r="P12" s="27" t="s">
         <v>49</v>
-      </c>
-      <c r="P12" s="27" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="24" x14ac:dyDescent="0.2">
       <c r="A13" s="33" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B13" s="34" t="s">
+        <v>50</v>
+      </c>
+      <c r="C13" s="35" t="s">
         <v>51</v>
-      </c>
-      <c r="C13" s="35" t="s">
-        <v>52</v>
       </c>
       <c r="D13" s="36">
         <v>2</v>
       </c>
       <c r="E13" s="37" t="s">
+        <v>52</v>
+      </c>
+      <c r="F13" s="37" t="s">
         <v>53</v>
-      </c>
-      <c r="F13" s="37" t="s">
-        <v>54</v>
       </c>
       <c r="G13" s="38">
         <v>10</v>
       </c>
       <c r="H13" s="33" t="s">
+        <v>54</v>
+      </c>
+      <c r="I13" s="39" t="s">
         <v>55</v>
-      </c>
-      <c r="I13" s="39" t="s">
-        <v>56</v>
       </c>
       <c r="J13" s="40">
         <v>0.01</v>
@@ -1477,7 +1490,7 @@
         <v>9.9</v>
       </c>
       <c r="L13" s="33" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="M13" s="41">
         <v>9</v>

</xml_diff>